<commit_message>
UPDATE: The cost prediction
</commit_message>
<xml_diff>
--- a/core/WBS成本向.xlsx
+++ b/core/WBS成本向.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\清风\Desktop\IT_project_management\IT_project_management\IT_project\IT_project_together\core\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A859F99-46FD-4A18-B21F-E61206DD3A14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20603" windowHeight="8495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="90">
   <si>
     <t>WBS</t>
   </si>
@@ -49,6 +43,24 @@
     <t>数据获取</t>
   </si>
   <si>
+    <t>阶段目标</t>
+  </si>
+  <si>
+    <t>人数/个</t>
+  </si>
+  <si>
+    <t>时间/日</t>
+  </si>
+  <si>
+    <t>成本预算/元</t>
+  </si>
+  <si>
+    <t>实际成本/元</t>
+  </si>
+  <si>
+    <t>差异/元</t>
+  </si>
+  <si>
     <t>安全保护</t>
   </si>
   <si>
@@ -61,9 +73,15 @@
     <t>1.2d</t>
   </si>
   <si>
+    <t>基本功能实现</t>
+  </si>
+  <si>
     <t>登录注册功能</t>
   </si>
   <si>
+    <t>核心功能实现</t>
+  </si>
+  <si>
     <t>2.1.1</t>
   </si>
   <si>
@@ -73,16 +91,28 @@
     <t>0.1d</t>
   </si>
   <si>
+    <t>第三方平台合作</t>
+  </si>
+  <si>
+    <t>未知</t>
+  </si>
+  <si>
     <t>2.1.2</t>
   </si>
   <si>
     <t>编写数据库CRUD</t>
   </si>
   <si>
+    <t>上线运营维护</t>
+  </si>
+  <si>
     <t>2.1.3</t>
   </si>
   <si>
     <t>Dao层调用</t>
+  </si>
+  <si>
+    <t>合计</t>
   </si>
   <si>
     <t>2.1.4</t>
@@ -259,8 +289,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,19 +306,157 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="4" tint="0.39997558519241921"/>
+      <color theme="4" tint="0.399975585192419"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,8 +475,200 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.05"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -581,11 +947,253 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -620,6 +1228,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -629,6 +1240,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -638,6 +1255,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -657,17 +1277,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -925,26 +1589,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="22.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5573770491803" style="1" customWidth="1"/>
     <col min="3" max="4" width="9" style="1"/>
+    <col min="7" max="7" width="15.2459016393443" customWidth="1"/>
+    <col min="10" max="10" width="10.6147540983607" customWidth="1"/>
+    <col min="11" max="11" width="11.8852459016393" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" ht="15.15" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -958,7 +1625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" ht="15.15" spans="1:4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -972,9 +1639,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" ht="15.15" spans="1:4">
       <c r="A3" s="6">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>6</v>
@@ -986,7 +1653,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="9">
         <v>1.2</v>
       </c>
@@ -999,111 +1666,229 @@
       <c r="D4" s="11">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="G4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" ht="15.15" spans="1:12">
+      <c r="A5" s="13">
         <v>1.3</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="14">
+      <c r="B5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="15">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="J5" s="17">
+        <v>180</v>
+      </c>
+      <c r="K5" s="17">
+        <v>200</v>
+      </c>
+      <c r="L5" s="17">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" ht="15.15" spans="1:12">
       <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D6" s="5">
         <v>180</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="G6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="J6" s="17">
+        <v>180</v>
+      </c>
+      <c r="K6" s="17">
+        <v>200</v>
+      </c>
+      <c r="L6" s="17">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="7" ht="15.15" spans="1:12">
+      <c r="A7" s="18">
         <v>2.1</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="17">
+      <c r="B7" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="20">
         <v>180</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G7" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17">
+        <v>6.4</v>
+      </c>
+      <c r="J7" s="17">
+        <v>15000</v>
+      </c>
+      <c r="K7" s="17">
+        <v>12000</v>
+      </c>
+      <c r="L7" s="17">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D8" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="17">
+        <v>28</v>
+      </c>
+      <c r="J8" s="17">
+        <v>2800</v>
+      </c>
+      <c r="K8" s="17">
+        <v>3000</v>
+      </c>
+      <c r="L8" s="17">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="9" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D9" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17">
+        <v>40</v>
+      </c>
+      <c r="J9" s="17">
+        <v>30000</v>
+      </c>
+      <c r="K9" s="17">
+        <v>28000</v>
+      </c>
+      <c r="L9" s="17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="9" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D10" s="11">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G10" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="21">
+        <v>4</v>
+      </c>
+      <c r="I10" s="21">
+        <v>76.9</v>
+      </c>
+      <c r="J10" s="21">
+        <v>48160</v>
+      </c>
+      <c r="K10" s="21">
+        <v>40400</v>
+      </c>
+      <c r="L10" s="21">
+        <v>4940</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="9" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D11" s="11">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="9" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>7</v>
@@ -1112,54 +1897,54 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="14">
+    <row r="13" spans="1:4">
+      <c r="A13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="15">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="3">
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D14" s="5">
         <v>15000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+    <row r="15" spans="1:4">
+      <c r="A15" s="18">
         <v>3.1</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="17">
+      <c r="B15" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="20">
         <v>800</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="9" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>7</v>
@@ -1168,12 +1953,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="9" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>7</v>
@@ -1182,288 +1967,288 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="20">
+    <row r="18" spans="1:4">
+      <c r="A18" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="24">
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+    <row r="19" spans="1:4">
+      <c r="A19" s="25">
         <v>3.2</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="23">
+      <c r="B19" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="27">
         <v>13200</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="6" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D20" s="8">
         <v>2000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D21" s="11">
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="9" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="D22" s="11">
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="19" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="24">
         <v>10000</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+    <row r="24" spans="1:4">
+      <c r="A24" s="18">
         <v>3.3</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="17">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="D25" s="11">
         <v>800</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="13" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="15">
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="3">
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D27" s="5">
         <v>2800</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="17">
+    <row r="28" spans="1:4">
+      <c r="A28" s="18">
+        <v>4.1</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="20">
         <v>1300</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="9" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="D29" s="11">
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="20">
+    <row r="30" spans="1:4">
+      <c r="A30" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="24">
         <v>1000</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+    <row r="31" spans="1:4">
+      <c r="A31" s="18">
         <v>4.2</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="17">
+      <c r="B31" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="20">
         <v>1500</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="9" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D32" s="11">
         <v>500</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="9" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D33" s="11">
         <v>500</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="14">
+    <row r="34" spans="1:4">
+      <c r="A34" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="15">
         <v>500</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="3">
         <v>5</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D35" s="5">
         <v>30000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="6">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D36" s="8">
         <v>20000</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12">
+    <row r="37" spans="1:4">
+      <c r="A37" s="13">
         <v>5.2</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="14">
+      <c r="B37" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="15">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>